<commit_message>
Remove Intvs from main model
</commit_message>
<xml_diff>
--- a/docs/ParsTable.xlsx
+++ b/docs/ParsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IndiaTB\IndTB_ACF\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936F14CA-0EEA-4DAF-9FE5-20207D0CB7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C700DA-53AC-4857-B260-A8C95D743595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="215">
   <si>
     <t>Parameter</t>
   </si>
@@ -343,9 +343,6 @@
     <t>\textit{Routine healthcare}</t>
   </si>
   <si>
-    <t>\textit{Active case-finding}</t>
-  </si>
-  <si>
     <t>\textbf{Parameter}</t>
   </si>
   <si>
@@ -656,6 +653,24 @@
   </si>
   <si>
     <t>Specificity, Xpert MTB/RIF</t>
+  </si>
+  <si>
+    <t>Prior/Value</t>
+  </si>
+  <si>
+    <t>Prop. seeking care from private sector</t>
+  </si>
+  <si>
+    <t>Prop. correctly diagnosed per visit, public</t>
+  </si>
+  <si>
+    <t>Prop.  correctly diagnosed per visit, private</t>
+  </si>
+  <si>
+    <t>Prop.  of TB recognised as DR-TB at point of diagnosis (public sector)</t>
+  </si>
+  <si>
+    <t>Prop. death during treatment period, first-line, DS</t>
   </si>
 </sst>
 </file>
@@ -707,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -724,11 +739,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -739,6 +798,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D692990D-2D58-4627-8701-2F5908D425D9}" name="Table3" displayName="Table3" ref="A46:D53" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="A46:D53" xr:uid="{D692990D-2D58-4627-8701-2F5908D425D9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FCB85AE9-BE4D-484A-8D18-99404DCFFFE5}" name="Parameter" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{06E6B94C-628B-49D8-BBB8-DA9B73814612}" name="Symbol" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A5E36643-AB75-4507-AB7C-2DB62D8A01E6}" name="Prior/Value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{494A7644-F1B5-43AE-80AA-F215EDF78412}" name="Source/note" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1503,7 +1575,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:D53"/>
+      <selection activeCell="D44" sqref="A29:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,16 +1588,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1539,13 +1611,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1553,13 +1625,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1567,13 +1639,13 @@
         <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1581,16 +1653,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,10 +1676,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>49</v>
@@ -1615,13 +1687,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>49</v>
@@ -1632,10 +1704,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>49</v>
@@ -1646,10 +1718,10 @@
         <v>60</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>49</v>
@@ -1660,16 +1732,16 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,13 +1752,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>51</v>
@@ -1697,49 +1769,49 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>54</v>
@@ -1750,64 +1822,64 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -1816,7 +1888,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>92</v>
@@ -1830,16 +1902,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,13 +1922,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>49</v>
@@ -1864,13 +1936,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>49</v>
@@ -1878,41 +1950,41 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>37</v>
+        <v>211</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>36</v>
+        <v>212</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>49</v>
@@ -1920,16 +1992,16 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>96</v>
+        <v>213</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,13 +2009,13 @@
         <v>80</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1951,13 +2023,13 @@
         <v>26</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1965,35 +2037,35 @@
         <v>27</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>87</v>
@@ -2004,155 +2076,159 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>214</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="D48" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B50" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="3">
+      <c r="C53" s="8">
         <v>1</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>162</v>
+      <c r="D53" s="8" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2161,5 +2237,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>